<commit_message>
Added comment in Excel on artificial data.
</commit_message>
<xml_diff>
--- a/data_epidemiological/Simulated Malaria Morbidty 2012 Week28-52.xlsx
+++ b/data_epidemiological/Simulated Malaria Morbidty 2012 Week28-52.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neko0001\Work\R_dev\epidemia-scripts-backstage\developer_only\20190324_datastash\data_epidemiological\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neko0001\Work\R_dev\epidemiar-demo\data_epidemiological\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,6 +16,136 @@
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Nekorchuk, Dawn M.</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nekorchuk, Dawn M.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Artificial data - not to be used for research or public health purposes.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nekorchuk, Dawn M.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Artificial data - not to be used for research or public health purposes.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nekorchuk, Dawn M.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Artificial data - not to be used for research or public health purposes.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nekorchuk, Dawn M.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Artificial data - not to be used for research or public health purposes.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nekorchuk, Dawn M.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Artificial data - not to be used for research or public health purposes.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -352,7 +482,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -367,6 +497,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -672,10 +815,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -41855,5 +42000,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>